<commit_message>
calibration files for IASC NO3_IBBCEAS
</commit_message>
<xml_diff>
--- a/IASC/NO3_IBBCEAS/NeLampSlitON.xlsx
+++ b/IASC/NO3_IBBCEAS/NeLampSlitON.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NO3_IBBCEAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{099CBC31-7542-47B3-A15F-F236A6D355CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{2A48DB35-5BA9-44F4-9036-3A39799FC9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
@@ -8605,8 +8605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O1025"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>